<commit_message>
add more tables and update
</commit_message>
<xml_diff>
--- a/data/excel_tables/2.2_other_party_orgs_info.xlsx
+++ b/data/excel_tables/2.2_other_party_orgs_info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="109">
   <si>
     <t>other_party_org_name</t>
   </si>
@@ -329,6 +329,18 @@
   </si>
   <si>
     <t>425c96b0-eaad-11ee-bce9-638f8e04ad34</t>
+  </si>
+  <si>
+    <t>9032f690-0182-11ef-938a-5514903835ea</t>
+  </si>
+  <si>
+    <t>a38ae5e0-0182-11ef-95c4-e7bfad33aba2</t>
+  </si>
+  <si>
+    <t>b2cb7830-0182-11ef-ae0a-87878d7061af</t>
+  </si>
+  <si>
+    <t>c5f838d0-0182-11ef-95c4-e7bfad33aba2</t>
   </si>
 </sst>
 </file>
@@ -686,7 +698,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2417,6 +2429,282 @@
         <v>104</v>
       </c>
     </row>
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
+        <v>42</v>
+      </c>
+      <c r="B76" t="s">
+        <v>79</v>
+      </c>
+      <c r="C76" t="s">
+        <v>84</v>
+      </c>
+      <c r="D76" t="s">
+        <v>86</v>
+      </c>
+      <c r="E76" t="s">
+        <v>92</v>
+      </c>
+      <c r="F76" t="s">
+        <v>96</v>
+      </c>
+      <c r="G76" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
+        <v>42</v>
+      </c>
+      <c r="B77" t="s">
+        <v>79</v>
+      </c>
+      <c r="C77" t="s">
+        <v>84</v>
+      </c>
+      <c r="D77" t="s">
+        <v>86</v>
+      </c>
+      <c r="E77" t="s">
+        <v>92</v>
+      </c>
+      <c r="F77" t="s">
+        <v>96</v>
+      </c>
+      <c r="G77" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
+        <v>43</v>
+      </c>
+      <c r="B78" t="s">
+        <v>80</v>
+      </c>
+      <c r="C78" t="s">
+        <v>84</v>
+      </c>
+      <c r="D78" t="s">
+        <v>86</v>
+      </c>
+      <c r="E78" t="s">
+        <v>92</v>
+      </c>
+      <c r="F78" t="s">
+        <v>96</v>
+      </c>
+      <c r="G78" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
+        <v>43</v>
+      </c>
+      <c r="B79" t="s">
+        <v>80</v>
+      </c>
+      <c r="C79" t="s">
+        <v>84</v>
+      </c>
+      <c r="D79" t="s">
+        <v>86</v>
+      </c>
+      <c r="E79" t="s">
+        <v>92</v>
+      </c>
+      <c r="F79" t="s">
+        <v>96</v>
+      </c>
+      <c r="G79" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
+        <v>43</v>
+      </c>
+      <c r="B80" t="s">
+        <v>80</v>
+      </c>
+      <c r="C80" t="s">
+        <v>82</v>
+      </c>
+      <c r="D80" t="s">
+        <v>86</v>
+      </c>
+      <c r="E80" t="s">
+        <v>92</v>
+      </c>
+      <c r="F80" t="s">
+        <v>96</v>
+      </c>
+      <c r="G80" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" t="s">
+        <v>43</v>
+      </c>
+      <c r="B81" t="s">
+        <v>80</v>
+      </c>
+      <c r="C81" t="s">
+        <v>82</v>
+      </c>
+      <c r="D81" t="s">
+        <v>86</v>
+      </c>
+      <c r="E81" t="s">
+        <v>92</v>
+      </c>
+      <c r="F81" t="s">
+        <v>96</v>
+      </c>
+      <c r="G81" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" t="s">
+        <v>42</v>
+      </c>
+      <c r="B82" t="s">
+        <v>79</v>
+      </c>
+      <c r="C82" t="s">
+        <v>82</v>
+      </c>
+      <c r="D82" t="s">
+        <v>86</v>
+      </c>
+      <c r="E82" t="s">
+        <v>92</v>
+      </c>
+      <c r="F82" t="s">
+        <v>96</v>
+      </c>
+      <c r="G82" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
+        <v>42</v>
+      </c>
+      <c r="B83" t="s">
+        <v>79</v>
+      </c>
+      <c r="C83" t="s">
+        <v>82</v>
+      </c>
+      <c r="D83" t="s">
+        <v>86</v>
+      </c>
+      <c r="E83" t="s">
+        <v>92</v>
+      </c>
+      <c r="F83" t="s">
+        <v>96</v>
+      </c>
+      <c r="G83" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>42</v>
+      </c>
+      <c r="B84" t="s">
+        <v>79</v>
+      </c>
+      <c r="C84" t="s">
+        <v>81</v>
+      </c>
+      <c r="D84" t="s">
+        <v>86</v>
+      </c>
+      <c r="E84" t="s">
+        <v>92</v>
+      </c>
+      <c r="F84" t="s">
+        <v>96</v>
+      </c>
+      <c r="G84" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
+        <v>43</v>
+      </c>
+      <c r="B85" t="s">
+        <v>80</v>
+      </c>
+      <c r="C85" t="s">
+        <v>81</v>
+      </c>
+      <c r="D85" t="s">
+        <v>86</v>
+      </c>
+      <c r="E85" t="s">
+        <v>92</v>
+      </c>
+      <c r="F85" t="s">
+        <v>96</v>
+      </c>
+      <c r="G85" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
+        <v>42</v>
+      </c>
+      <c r="B86" t="s">
+        <v>79</v>
+      </c>
+      <c r="C86" t="s">
+        <v>83</v>
+      </c>
+      <c r="D86" t="s">
+        <v>86</v>
+      </c>
+      <c r="E86" t="s">
+        <v>92</v>
+      </c>
+      <c r="F86" t="s">
+        <v>96</v>
+      </c>
+      <c r="G86" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>43</v>
+      </c>
+      <c r="B87" t="s">
+        <v>80</v>
+      </c>
+      <c r="C87" t="s">
+        <v>83</v>
+      </c>
+      <c r="D87" t="s">
+        <v>86</v>
+      </c>
+      <c r="E87" t="s">
+        <v>92</v>
+      </c>
+      <c r="F87" t="s">
+        <v>96</v>
+      </c>
+      <c r="G87" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>